<commit_message>
added stories 27 and 36
</commit_message>
<xml_diff>
--- a/SSW-555--Project 04-Sprint4/Team_DDGK_Report.xlsx
+++ b/SSW-555--Project 04-Sprint4/Team_DDGK_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krutarth\Desktop\SSW-555-DDGK-master\SSW-555--Project 04-Sprint4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhaval\Downloads\SSW-555-DDGK-master (4)\SSW-555-DDGK-master\SSW-555--Project 04-Sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF1C35E-698C-4313-BA55-38820F5C610C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25CFC65-862E-43A9-BDE6-7C1F68B9FA83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="290">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -919,6 +919,30 @@
   </si>
   <si>
     <t>197-201</t>
+  </si>
+  <si>
+    <t>US27_List_individual_current_ages</t>
+  </si>
+  <si>
+    <t>US36_List_recent_deaths</t>
+  </si>
+  <si>
+    <t>809-817</t>
+  </si>
+  <si>
+    <t>822-831</t>
+  </si>
+  <si>
+    <t>test_US27</t>
+  </si>
+  <si>
+    <t>test_US36</t>
+  </si>
+  <si>
+    <t>223-229</t>
+  </si>
+  <si>
+    <t>231-235</t>
   </si>
 </sst>
 </file>
@@ -929,7 +953,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -2568,7 +2592,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.69140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
@@ -2577,7 +2601,7 @@
     <col min="5" max="5" width="42.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="24" customHeight="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2594,7 +2618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1">
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>187</v>
       </c>
@@ -2611,7 +2635,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24" customHeight="1">
+    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -2628,7 +2652,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1">
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2645,7 +2669,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="24" customHeight="1">
+    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -2662,7 +2686,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="24" customHeight="1">
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
@@ -2691,11 +2715,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="56" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="56" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28" defaultRowHeight="67" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="28" defaultRowHeight="67" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" style="50"/>
     <col min="2" max="2" width="46.3046875" style="50" bestFit="1" customWidth="1"/>
@@ -2705,7 +2729,7 @@
     <col min="12" max="16384" width="28" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="67" customHeight="1">
+    <row r="1" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
         <v>3</v>
       </c>
@@ -2753,12 +2777,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="67" customHeight="1">
+    <row r="2" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>190</v>
@@ -2772,17 +2796,35 @@
       <c r="F2" s="50">
         <v>30</v>
       </c>
+      <c r="G2" s="50">
+        <v>12</v>
+      </c>
+      <c r="H2" s="50">
+        <v>25</v>
+      </c>
       <c r="I2" s="50" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="J2" s="50" t="s">
         <v>227</v>
       </c>
+      <c r="K2" s="50" t="s">
+        <v>282</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>284</v>
+      </c>
       <c r="N2" s="50" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="67" customHeight="1">
+      <c r="O2" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="51" t="str">
         <f>Stories!A37</f>
         <v>US36</v>
@@ -2803,17 +2845,35 @@
       <c r="F3" s="50">
         <v>55</v>
       </c>
+      <c r="G3" s="50">
+        <v>13</v>
+      </c>
+      <c r="H3" s="50">
+        <v>20</v>
+      </c>
       <c r="I3" s="50" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="J3" s="50" t="s">
         <v>227</v>
       </c>
+      <c r="K3" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="L3" s="50" t="s">
+        <v>285</v>
+      </c>
       <c r="N3" s="50" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="67" customHeight="1">
+      <c r="O3" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="P3" s="50" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
         <v>136</v>
       </c>
@@ -2860,7 +2920,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="67" customHeight="1">
+    <row r="5" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="50" t="s">
         <v>146</v>
       </c>
@@ -2907,7 +2967,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="67" customHeight="1">
+    <row r="6" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="51" t="str">
         <f>Stories!A39</f>
         <v>US38</v>
@@ -2956,7 +3016,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="67" customHeight="1">
+    <row r="7" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="51" t="str">
         <f>Stories!A40</f>
         <v>US39</v>
@@ -3005,7 +3065,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="67" customHeight="1">
+    <row r="8" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="51" t="s">
         <v>141</v>
       </c>
@@ -3034,7 +3094,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="67" customHeight="1">
+    <row r="9" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="51" t="s">
         <v>144</v>
       </c>
@@ -3063,77 +3123,78 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="67" customHeight="1">
+    <row r="13" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="67" customHeight="1">
+    <row r="14" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="46"/>
     </row>
-    <row r="15" spans="1:16" ht="67" customHeight="1">
+    <row r="15" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="67" customHeight="1">
+    <row r="16" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="54" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="67" customHeight="1">
+    <row r="17" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="54" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="67" customHeight="1">
+    <row r="18" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="54" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="67" customHeight="1">
+    <row r="19" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="54" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="67" customHeight="1">
+    <row r="20" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="54"/>
     </row>
-    <row r="21" spans="2:2" ht="67" customHeight="1">
+    <row r="21" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="54"/>
     </row>
-    <row r="22" spans="2:2" ht="67" customHeight="1">
+    <row r="22" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="54"/>
     </row>
-    <row r="23" spans="2:2" ht="67" customHeight="1">
+    <row r="23" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="46" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="67" customHeight="1">
+    <row r="24" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="54" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="67" customHeight="1">
+    <row r="25" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="54" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="67" customHeight="1">
+    <row r="26" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="67" customHeight="1">
+    <row r="27" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="54"/>
     </row>
-    <row r="28" spans="2:2" ht="67" customHeight="1">
+    <row r="28" spans="2:2" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="54"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3145,12 +3206,12 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15234375" defaultRowHeight="19" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.15234375" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>29</v>
       </c>
@@ -3167,7 +3228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19" customHeight="1">
+    <row r="2" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56">
         <v>1</v>
       </c>
@@ -3184,7 +3245,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19" customHeight="1">
+    <row r="3" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>1</v>
       </c>
@@ -3201,7 +3262,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19" customHeight="1">
+    <row r="4" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>1</v>
       </c>
@@ -3218,7 +3279,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" customHeight="1">
+    <row r="5" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>1</v>
       </c>
@@ -3235,7 +3296,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19" customHeight="1">
+    <row r="6" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>1</v>
       </c>
@@ -3252,7 +3313,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19" customHeight="1">
+    <row r="7" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>1</v>
       </c>
@@ -3269,7 +3330,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19" customHeight="1">
+    <row r="8" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>1</v>
       </c>
@@ -3286,7 +3347,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19" customHeight="1">
+    <row r="9" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>1</v>
       </c>
@@ -3303,7 +3364,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19" customHeight="1">
+    <row r="10" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56">
         <v>2</v>
       </c>
@@ -3320,7 +3381,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19" customHeight="1">
+    <row r="11" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="56">
         <v>2</v>
       </c>
@@ -3337,7 +3398,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19" customHeight="1">
+    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56">
         <v>2</v>
       </c>
@@ -3354,7 +3415,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19" customHeight="1">
+    <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56">
         <v>2</v>
       </c>
@@ -3371,7 +3432,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19" customHeight="1">
+    <row r="14" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="56">
         <v>2</v>
       </c>
@@ -3388,7 +3449,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19" customHeight="1">
+    <row r="15" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="56">
         <v>2</v>
       </c>
@@ -3405,7 +3466,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19" customHeight="1">
+    <row r="16" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="56">
         <v>2</v>
       </c>
@@ -3422,7 +3483,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="19" customHeight="1">
+    <row r="17" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="56">
         <v>2</v>
       </c>
@@ -3439,7 +3500,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19" customHeight="1">
+    <row r="18" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="56">
         <v>3</v>
       </c>
@@ -3456,7 +3517,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19" customHeight="1">
+    <row r="19" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="56">
         <v>3</v>
       </c>
@@ -3473,7 +3534,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19" customHeight="1">
+    <row r="20" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="56">
         <v>3</v>
       </c>
@@ -3490,7 +3551,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19" customHeight="1">
+    <row r="21" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="56">
         <v>3</v>
       </c>
@@ -3507,7 +3568,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="19" customHeight="1">
+    <row r="22" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="56">
         <v>3</v>
       </c>
@@ -3524,7 +3585,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="19" customHeight="1">
+    <row r="23" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="56">
         <v>3</v>
       </c>
@@ -3541,7 +3602,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19" customHeight="1">
+    <row r="24" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="56">
         <v>3</v>
       </c>
@@ -3558,7 +3619,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="19" customHeight="1">
+    <row r="25" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="56">
         <v>3</v>
       </c>
@@ -3575,7 +3636,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="19" customHeight="1">
+    <row r="26" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="56">
         <v>4</v>
       </c>
@@ -3592,7 +3653,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="19" customHeight="1">
+    <row r="27" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="56">
         <v>4</v>
       </c>
@@ -3609,7 +3670,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="19" customHeight="1">
+    <row r="28" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="56">
         <v>4</v>
       </c>
@@ -3626,7 +3687,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="19" customHeight="1">
+    <row r="29" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="56">
         <v>4</v>
       </c>
@@ -3643,7 +3704,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="19" customHeight="1">
+    <row r="30" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="56">
         <v>4</v>
       </c>
@@ -3660,7 +3721,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="19" customHeight="1">
+    <row r="31" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="56">
         <v>4</v>
       </c>
@@ -3677,7 +3738,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="19" customHeight="1">
+    <row r="32" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56">
         <v>4</v>
       </c>
@@ -3694,7 +3755,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="19" customHeight="1">
+    <row r="33" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="56">
         <v>4</v>
       </c>
@@ -3711,10 +3772,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="19" customHeight="1">
+    <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E34" s="30"/>
     </row>
-    <row r="35" spans="1:5" ht="19" customHeight="1">
+    <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E35" s="30"/>
     </row>
   </sheetData>
@@ -3730,7 +3791,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3744,7 +3805,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.84375" style="2"/>
     <col min="2" max="2" width="9.4609375" customWidth="1"/>
@@ -3754,37 +3815,37 @@
     <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>159</v>
       </c>
@@ -3807,7 +3868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -3823,7 +3884,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -3848,7 +3909,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>162</v>
       </c>
@@ -3874,7 +3935,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>163</v>
       </c>
@@ -3899,7 +3960,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>164</v>
       </c>
@@ -3939,7 +4000,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.69140625" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.69140625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.15234375" style="1" bestFit="1" customWidth="1"/>
@@ -3959,7 +4020,7 @@
     <col min="17" max="17" width="10.15234375" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1">
+    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4006,7 +4067,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18" customHeight="1">
+    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
         <v>112</v>
       </c>
@@ -4045,7 +4106,7 @@
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
     </row>
-    <row r="3" spans="1:17" ht="18" customHeight="1">
+    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41" t="s">
         <v>113</v>
       </c>
@@ -4080,7 +4141,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1">
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="41" t="s">
         <v>114</v>
       </c>
@@ -4115,7 +4176,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" customHeight="1">
+    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>115</v>
       </c>
@@ -4150,7 +4211,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1">
+    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41" t="s">
         <v>116</v>
       </c>
@@ -4185,7 +4246,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18" customHeight="1">
+    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
         <v>117</v>
       </c>
@@ -4220,7 +4281,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18" customHeight="1">
+    <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
         <v>118</v>
       </c>
@@ -4259,7 +4320,7 @@
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
     </row>
-    <row r="9" spans="1:17" ht="18" customHeight="1">
+    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
         <v>119</v>
       </c>
@@ -4294,52 +4355,52 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18" customHeight="1">
+    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="30"/>
       <c r="G10">
         <f>SUM(G2:G9)</f>
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18" customHeight="1">
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" customHeight="1">
+    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1">
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="18" customHeight="1">
+    <row r="17" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="42" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="18" customHeight="1">
+    <row r="18" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="42" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="18" customHeight="1">
+    <row r="19" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="42" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="18" customHeight="1">
+    <row r="20" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="18" customHeight="1">
+    <row r="21" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="42" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="18" customHeight="1">
+    <row r="22" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="42" t="s">
         <v>215</v>
       </c>
@@ -4359,7 +4420,7 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.84375" style="2"/>
     <col min="2" max="2" width="16.69140625" customWidth="1"/>
@@ -4369,7 +4430,7 @@
     <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4389,7 +4450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42046</v>
       </c>
@@ -4409,7 +4470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42061</v>
       </c>
@@ -4431,7 +4492,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42087</v>
       </c>
@@ -4452,7 +4513,7 @@
         <v>53.142857142857139</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42101</v>
       </c>
@@ -4488,13 +4549,13 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="25.69140625" customWidth="1"/>
     <col min="9" max="9" width="13.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4523,7 +4584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>120</v>
       </c>
@@ -4552,7 +4613,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>121</v>
       </c>
@@ -4581,7 +4642,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>122</v>
       </c>
@@ -4610,7 +4671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>123</v>
       </c>
@@ -4639,7 +4700,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>124</v>
       </c>
@@ -4668,7 +4729,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>125</v>
       </c>
@@ -4697,7 +4758,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>126</v>
       </c>
@@ -4726,7 +4787,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>142</v>
       </c>
@@ -4755,68 +4816,68 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="27">
+    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B15" s="42" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="42" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="42" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="27">
+    <row r="18" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B18" s="42" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="42" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="27">
+    <row r="20" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B20" s="42" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="42"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="42" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="42" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="27">
+    <row r="25" spans="2:2" ht="27" x14ac:dyDescent="0.3">
       <c r="B25" s="42" t="s">
         <v>224</v>
       </c>
@@ -4836,7 +4897,7 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="60"/>
     <col min="2" max="2" width="27" style="60" bestFit="1" customWidth="1"/>
@@ -4846,7 +4907,7 @@
     <col min="12" max="16384" width="19" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
@@ -4893,7 +4954,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1">
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="61" t="s">
         <v>127</v>
       </c>
@@ -4940,7 +5001,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" customHeight="1">
+    <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="61" t="s">
         <v>129</v>
       </c>
@@ -4987,7 +5048,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1">
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61" t="s">
         <v>130</v>
       </c>
@@ -5034,7 +5095,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1">
+    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>131</v>
       </c>
@@ -5081,7 +5142,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1">
+    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61" t="s">
         <v>132</v>
       </c>
@@ -5128,7 +5189,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1">
+    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="61" t="s">
         <v>133</v>
       </c>
@@ -5175,7 +5236,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1">
+    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="61" t="s">
         <v>134</v>
       </c>
@@ -5222,7 +5283,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1">
+    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="61" t="s">
         <v>135</v>
       </c>
@@ -5269,70 +5330,70 @@
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="52" customHeight="1">
+    <row r="14" spans="1:15" ht="52" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="59" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="61" customHeight="1">
+    <row r="15" spans="1:15" ht="61" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="62" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1">
+    <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="59" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="3:3" ht="30" customHeight="1">
+    <row r="17" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="62" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="3:3" ht="30" customHeight="1">
+    <row r="18" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="62" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="3:3" ht="30" customHeight="1">
+    <row r="19" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="62" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="3:3" ht="30" customHeight="1">
+    <row r="20" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="62" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="21" spans="3:3" ht="30" customHeight="1">
+    <row r="21" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="62" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="30" customHeight="1">
+    <row r="22" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="62" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="30" customHeight="1">
+    <row r="23" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="62"/>
     </row>
-    <row r="24" spans="3:3" ht="30" customHeight="1">
+    <row r="24" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="59" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="3:3" ht="30" customHeight="1">
+    <row r="25" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="62" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="3:3" ht="30" customHeight="1">
+    <row r="26" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="62" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="3:3" ht="30" customHeight="1">
+    <row r="27" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="62" t="s">
         <v>224</v>
       </c>
@@ -5348,17 +5409,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView zoomScale="61" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A28" zoomScale="86" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
@@ -5369,7 +5430,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>112</v>
       </c>
@@ -5384,7 +5445,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>113</v>
       </c>
@@ -5399,7 +5460,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>114</v>
       </c>
@@ -5414,7 +5475,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>115</v>
       </c>
@@ -5429,7 +5490,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>116</v>
       </c>
@@ -5440,7 +5501,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>117</v>
       </c>
@@ -5451,7 +5512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
         <v>118</v>
       </c>
@@ -5462,7 +5523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>119</v>
       </c>
@@ -5473,7 +5534,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>120</v>
       </c>
@@ -5484,7 +5545,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>121</v>
       </c>
@@ -5495,7 +5556,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>122</v>
       </c>
@@ -5506,7 +5567,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>123</v>
       </c>
@@ -5517,7 +5578,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60">
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>124</v>
       </c>
@@ -5528,7 +5589,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>125</v>
       </c>
@@ -5539,7 +5600,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>126</v>
       </c>
@@ -5550,7 +5611,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>127</v>
       </c>
@@ -5561,7 +5622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>128</v>
       </c>
@@ -5572,7 +5633,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="35" t="s">
         <v>129</v>
       </c>
@@ -5583,7 +5644,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>130</v>
       </c>
@@ -5594,7 +5655,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>131</v>
       </c>
@@ -5605,7 +5666,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>132</v>
       </c>
@@ -5616,7 +5677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>133</v>
       </c>
@@ -5627,7 +5688,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>134</v>
       </c>
@@ -5638,7 +5699,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>135</v>
       </c>
@@ -5649,7 +5710,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>136</v>
       </c>
@@ -5660,7 +5721,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>137</v>
       </c>
@@ -5671,7 +5732,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>138</v>
       </c>
@@ -5682,7 +5743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>139</v>
       </c>
@@ -5693,7 +5754,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>140</v>
       </c>
@@ -5704,7 +5765,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>141</v>
       </c>
@@ -5715,7 +5776,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="39" t="s">
         <v>142</v>
       </c>
@@ -5726,7 +5787,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="23" customHeight="1">
+    <row r="33" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>143</v>
       </c>
@@ -5737,7 +5798,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -5748,7 +5809,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -5759,7 +5820,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>146</v>
       </c>
@@ -5770,7 +5831,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -5781,7 +5842,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>148</v>
       </c>
@@ -5792,7 +5853,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" s="39" t="s">
         <v>149</v>
       </c>
@@ -5803,7 +5864,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" s="39" t="s">
         <v>150</v>
       </c>
@@ -5814,7 +5875,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -5825,7 +5886,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>152</v>
       </c>
@@ -5836,7 +5897,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>153</v>
       </c>

</xml_diff>